<commit_message>
Add Excel portfolio project file
</commit_message>
<xml_diff>
--- a/MY EXCEL PORTFOLIO PROJECT.xlsx
+++ b/MY EXCEL PORTFOLIO PROJECT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nivif\Desktop\DA CLASS DOCS\EXCEL MAIN PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B1ECD8-A47F-4536-8331-F6E7B918D56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D44750B-0E9F-4154-9618-24F2A7131F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BAA1F89B-8E14-426D-BAB3-40AA3A9B4E7E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="54" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -6859,6 +6859,9 @@
       <c:pivotFmt>
         <c:idx val="14"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -9358,6 +9361,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -9376,6 +9384,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -9394,6 +9407,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -9412,6 +9430,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -9430,6 +9453,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -9448,6 +9476,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -9466,6 +9499,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-84F7-4AA2-8AD8-354CC536979C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -17688,7 +17726,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D69B3A66-A0C0-46EF-9B56-319C3FAD29B0}" name="Totalsales" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="9">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D69B3A66-A0C0-46EF-9B56-319C3FAD29B0}" name="Totalsales" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="9">
   <location ref="A3:F57" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -18232,7 +18270,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8996856B-3581-4547-945E-0C7A30F0A863}" name="Totalsales" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="17">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8996856B-3581-4547-945E-0C7A30F0A863}" name="Totalsales" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="17">
   <location ref="A3:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -18682,7 +18720,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF484BDC-CDDB-4113-9409-4415C9A947FD}" name="Totalsales" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="18">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF484BDC-CDDB-4113-9409-4415C9A947FD}" name="Totalsales" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="5" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="18">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="21">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -19785,7 +19823,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>

</xml_diff>